<commit_message>
발표자료, use-case, activity diagram 수정
</commit_message>
<xml_diff>
--- a/문서/회의록, 제안서/간트 차트.xlsx
+++ b/문서/회의록, 제안서/간트 차트.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyungsook\Desktop\쑥\2019 2학기\소프트웨어 설계\팀프로젝트\SD_2019_2_team7\문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyungsook\Desktop\쑥\2019 2학기\소프트웨어 설계\팀프로젝트\SD_2019_2_team7\문서\회의록, 제안서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B3805-DE6C-4A04-A57A-F73A88B14095}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD20F25C-612D-42E0-885A-15DE48E54135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A5335E2C-64F0-4936-B28B-08D34DEC03C8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{A5335E2C-64F0-4936-B28B-08D34DEC03C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -475,6 +475,33 @@
       </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -482,7 +509,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </left>
       <right/>
       <top/>
@@ -490,27 +541,116 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -520,10 +660,95 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -536,15 +761,30 @@
         <color theme="0" tint="-0.499984740745262"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -552,12 +792,197 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -566,120 +991,35 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -700,7 +1040,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,242 +1059,287 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="51" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="52" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="53" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1274,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9CE2A9-33F4-4BD6-830E-6BE33B2B69F5}">
-  <dimension ref="B3:X37"/>
+  <dimension ref="B2:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1290,48 +1675,49 @@
     <col min="10" max="10" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="77" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="81" t="s">
+      <c r="F3" s="70"/>
+      <c r="G3" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="81" t="s">
+      <c r="H3" s="71"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="81" t="s">
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="80" t="s">
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="81"/>
-      <c r="V3" s="82"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="74"/>
       <c r="W3" s="14"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B4" s="6"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="40" t="s">
+      <c r="E4" s="63"/>
+      <c r="F4" s="62" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1379,35 +1765,35 @@
       <c r="U4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="76" t="s">
         <v>24</v>
       </c>
       <c r="W4" s="13"/>
       <c r="X4" s="12"/>
     </row>
     <row r="5" spans="2:24" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="36"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18"/>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>33</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="22" t="s">
         <v>34</v>
       </c>
       <c r="N5" s="18"/>
@@ -1417,34 +1803,34 @@
       <c r="R5" s="17"/>
       <c r="S5" s="18"/>
       <c r="T5" s="19"/>
-      <c r="U5" s="23" t="s">
+      <c r="U5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="24" t="s">
+      <c r="V5" s="78" t="s">
         <v>43</v>
       </c>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
     </row>
     <row r="6" spans="2:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="47"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="38"/>
       <c r="N6" s="10"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1452,21 +1838,22 @@
       <c r="R6" s="7"/>
       <c r="S6" s="10"/>
       <c r="T6" s="16"/>
-      <c r="V6" s="3"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="80"/>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
     </row>
     <row r="7" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="75"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="35" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="49"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="7"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7"/>
@@ -1481,22 +1868,22 @@
       <c r="S7" s="10"/>
       <c r="T7" s="16"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="4"/>
+      <c r="V7" s="82"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
     <row r="8" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="75"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="35" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="49"/>
+      <c r="H8" s="40"/>
       <c r="I8" s="10"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1510,26 +1897,26 @@
       <c r="S8" s="10"/>
       <c r="T8" s="16"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="4"/>
+      <c r="V8" s="82"/>
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
     </row>
     <row r="9" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="75"/>
-      <c r="C9" s="79" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="42"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -1541,25 +1928,25 @@
       <c r="S9" s="10"/>
       <c r="T9" s="16"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="4"/>
+      <c r="V9" s="82"/>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
     </row>
     <row r="10" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="75"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="30" t="s">
+      <c r="B10" s="81"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="42"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="4"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="49"/>
+      <c r="K10" s="40"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="4"/>
@@ -1570,27 +1957,27 @@
       <c r="S10" s="10"/>
       <c r="T10" s="16"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="4"/>
+      <c r="V10" s="82"/>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="75"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="30" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="42"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="4"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="67"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
       <c r="N11" s="4"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -1599,51 +1986,51 @@
       <c r="S11" s="10"/>
       <c r="T11" s="16"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="4"/>
+      <c r="V11" s="82"/>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
     <row r="12" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="25"/>
+      <c r="E12" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
       <c r="I12" s="3"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="52"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="43"/>
       <c r="R12" s="20"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="68"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="56"/>
       <c r="U12" s="20"/>
-      <c r="V12" s="3"/>
+      <c r="V12" s="80"/>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
     </row>
     <row r="13" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="75"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="35" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="4"/>
@@ -1651,30 +2038,30 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="51"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="10"/>
       <c r="T13" s="16"/>
       <c r="U13" s="7"/>
-      <c r="V13" s="4"/>
+      <c r="V13" s="82"/>
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
     </row>
     <row r="14" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="75"/>
-      <c r="C14" s="79" t="s">
+      <c r="B14" s="81"/>
+      <c r="C14" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="42"/>
+      <c r="F14" s="33"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="4"/>
@@ -1684,26 +2071,26 @@
       <c r="M14" s="7"/>
       <c r="N14" s="4"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="49"/>
+      <c r="P14" s="40"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="10"/>
       <c r="T14" s="16"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="4"/>
+      <c r="V14" s="82"/>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
     </row>
     <row r="15" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="75"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="30" t="s">
+      <c r="B15" s="81"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="42"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="4"/>
@@ -1713,28 +2100,28 @@
       <c r="M15" s="7"/>
       <c r="N15" s="4"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="49"/>
+      <c r="P15" s="40"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="10"/>
       <c r="T15" s="16"/>
       <c r="U15" s="7"/>
-      <c r="V15" s="4"/>
+      <c r="V15" s="82"/>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
     <row r="16" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="75"/>
-      <c r="C16" s="79" t="s">
+      <c r="B16" s="81"/>
+      <c r="C16" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="42"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="4"/>
@@ -1745,82 +2132,82 @@
       <c r="N16" s="4"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
-      <c r="Q16" s="49"/>
+      <c r="Q16" s="40"/>
       <c r="R16" s="7"/>
       <c r="S16" s="10"/>
       <c r="T16" s="16"/>
       <c r="U16" s="7"/>
-      <c r="V16" s="4"/>
+      <c r="V16" s="82"/>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
     </row>
     <row r="17" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="76"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="30" t="s">
+      <c r="B17" s="83"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="43"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="64"/>
+      <c r="I17" s="52"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="64"/>
+      <c r="N17" s="52"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="49"/>
+      <c r="Q17" s="40"/>
       <c r="R17" s="1"/>
       <c r="S17" s="11"/>
-      <c r="T17" s="22"/>
+      <c r="T17" s="21"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="64"/>
+      <c r="V17" s="84"/>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
     </row>
     <row r="18" spans="2:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="63" t="s">
+      <c r="D18" s="25"/>
+      <c r="E18" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="65"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="52"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="85"/>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
     </row>
     <row r="19" spans="2:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="75"/>
-      <c r="C19" s="42" t="s">
+      <c r="B19" s="81"/>
+      <c r="C19" s="33" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="73" t="s">
+      <c r="E19" s="60" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="4"/>
@@ -1832,24 +2219,24 @@
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="58"/>
-      <c r="S19" s="59"/>
-      <c r="T19" s="59"/>
-      <c r="U19" s="59"/>
-      <c r="V19" s="53"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="86"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B20" s="75"/>
-      <c r="C20" s="42" t="s">
+      <c r="B20" s="81"/>
+      <c r="C20" s="33" t="s">
         <v>48</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="60" t="s">
         <v>52</v>
       </c>
       <c r="F20" s="4"/>
@@ -1861,22 +2248,22 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="57"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="55"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="71"/>
-      <c r="U20" s="71"/>
-      <c r="V20" s="54"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="59"/>
+      <c r="V20" s="87"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B21" s="75"/>
-      <c r="C21" s="42" t="s">
+      <c r="B21" s="81"/>
+      <c r="C21" s="33" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="73" t="s">
+      <c r="E21" s="60" t="s">
         <v>53</v>
       </c>
       <c r="F21" s="4"/>
@@ -1889,20 +2276,20 @@
       <c r="M21" s="7"/>
       <c r="N21" s="4"/>
       <c r="O21" s="7"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="59"/>
-      <c r="U21" s="59"/>
-      <c r="V21" s="53"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="86"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B22" s="76"/>
-      <c r="C22" s="43" t="s">
+      <c r="B22" s="83"/>
+      <c r="C22" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="64"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="5" t="s">
         <v>54</v>
       </c>
@@ -1915,47 +2302,47 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="4"/>
-      <c r="O22" s="57"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="71"/>
-      <c r="T22" s="70"/>
-      <c r="U22" s="70"/>
-      <c r="V22" s="72"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="88"/>
     </row>
-    <row r="23" spans="2:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="27" t="s">
+    <row r="23" spans="2:24" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="34" t="s">
+      <c r="C23" s="90"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="43"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="45"/>
-      <c r="V23" s="52"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="94"/>
+      <c r="P23" s="94"/>
+      <c r="Q23" s="94"/>
+      <c r="R23" s="94"/>
+      <c r="S23" s="97"/>
+      <c r="T23" s="98"/>
+      <c r="U23" s="98"/>
+      <c r="V23" s="99"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.4">
       <c r="L27" s="8"/>
     </row>
     <row r="36" spans="13:13" x14ac:dyDescent="0.4">
-      <c r="M36" s="29"/>
+      <c r="M36" s="23"/>
     </row>
     <row r="37" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M37" s="7"/>

</xml_diff>